<commit_message>
Actualización de formato EXCEL
</commit_message>
<xml_diff>
--- a/templates/Surveys.xlsx
+++ b/templates/Surveys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\project-ssm-back\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858E982B-45B2-432F-B436-DCCAD9847821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A501FC8-CE7D-4A59-9782-68A95AC5A0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EPS" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="67">
   <si>
     <t>Nombre de la EPS</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>edad</t>
   </si>
 </sst>
 </file>
@@ -851,36 +854,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB33"/>
+  <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="52"/>
+    <col min="1" max="1" width="7.46484375" style="52" customWidth="1"/>
     <col min="2" max="2" width="25.59765625" style="43" customWidth="1"/>
     <col min="3" max="3" width="25.59765625" style="18" customWidth="1"/>
     <col min="4" max="4" width="17.53125" style="19" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="20" customWidth="1"/>
     <col min="6" max="6" width="19.06640625" style="18" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="9.06640625" style="18"/>
-    <col min="9" max="9" width="16" style="20" customWidth="1"/>
-    <col min="10" max="10" width="46.6640625" style="18" customWidth="1"/>
-    <col min="11" max="11" width="21.59765625" style="19" customWidth="1"/>
-    <col min="12" max="12" width="24.796875" style="19" customWidth="1"/>
-    <col min="13" max="13" width="9.06640625" style="20"/>
-    <col min="14" max="14" width="9.6640625" style="20" customWidth="1"/>
-    <col min="15" max="22" width="9.06640625" style="20"/>
-    <col min="23" max="24" width="9.9296875" style="20" customWidth="1"/>
-    <col min="25" max="25" width="9.06640625" style="20"/>
-    <col min="26" max="16384" width="9.06640625" style="3"/>
+    <col min="8" max="9" width="9.06640625" style="18"/>
+    <col min="10" max="10" width="16" style="20" customWidth="1"/>
+    <col min="11" max="11" width="46.6640625" style="18" customWidth="1"/>
+    <col min="12" max="12" width="21.59765625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="24.796875" style="19" customWidth="1"/>
+    <col min="14" max="14" width="9.06640625" style="20"/>
+    <col min="15" max="15" width="9.6640625" style="20" customWidth="1"/>
+    <col min="16" max="23" width="9.06640625" style="20"/>
+    <col min="24" max="25" width="9.9296875" style="20" customWidth="1"/>
+    <col min="26" max="26" width="9.06640625" style="20"/>
+    <col min="27" max="16384" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="164" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:29" ht="164" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="51"/>
       <c r="B1" s="40"/>
       <c r="C1" s="12"/>
@@ -890,57 +893,58 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>1</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>2</v>
       </c>
       <c r="N1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AC1" s="2"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A2" s="53" t="s">
         <v>65</v>
       </c>
@@ -966,97 +970,100 @@
         <v>20</v>
       </c>
       <c r="I2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="K2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="17">
+      <c r="L2" s="17">
         <v>1</v>
       </c>
-      <c r="L2" s="17">
+      <c r="M2" s="17">
         <v>2</v>
       </c>
-      <c r="M2" s="17">
+      <c r="N2" s="17">
         <v>3</v>
       </c>
-      <c r="N2" s="17">
+      <c r="O2" s="17">
         <v>4</v>
       </c>
-      <c r="O2" s="17">
+      <c r="P2" s="17">
         <v>5</v>
       </c>
-      <c r="P2" s="17">
+      <c r="Q2" s="17">
         <v>6</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="R2" s="17">
         <v>7</v>
       </c>
-      <c r="R2" s="17">
+      <c r="S2" s="17">
         <v>8</v>
       </c>
-      <c r="S2" s="17">
+      <c r="T2" s="17">
         <v>9</v>
       </c>
-      <c r="T2" s="17">
+      <c r="U2" s="17">
         <v>10</v>
       </c>
-      <c r="U2" s="17">
+      <c r="V2" s="17">
         <v>11</v>
       </c>
-      <c r="V2" s="17">
+      <c r="W2" s="17">
         <v>12</v>
       </c>
-      <c r="W2" s="17" t="s">
+      <c r="X2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="17" t="s">
+      <c r="Y2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" s="17">
+      <c r="Z2" s="17">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B3" s="42"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B4" s="42"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B5" s="42"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B6" s="42"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B7" s="42"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B8" s="42"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B9" s="42"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B10" s="42"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B11" s="42"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B12" s="42"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B13" s="42"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B14" s="42"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B15" s="42"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B16" s="42"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">
@@ -1119,9 +1126,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -1136,22 +1143,23 @@
     <col min="6" max="6" width="9" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.86328125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.46484375" style="10" customWidth="1"/>
-    <col min="10" max="10" width="18" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" style="9" customWidth="1"/>
-    <col min="13" max="13" width="9.796875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="24.3984375" style="9" customWidth="1"/>
-    <col min="15" max="15" width="18.3984375" style="9" customWidth="1"/>
-    <col min="16" max="16" width="18" style="9" customWidth="1"/>
-    <col min="17" max="17" width="25.06640625" style="9" customWidth="1"/>
-    <col min="18" max="18" width="10.59765625" style="11" customWidth="1"/>
-    <col min="19" max="19" width="5.59765625" style="10" customWidth="1"/>
-    <col min="20" max="20" width="9.796875" style="9" customWidth="1"/>
-    <col min="21" max="16384" width="9.06640625" style="3"/>
+    <col min="9" max="9" width="6" style="9" customWidth="1"/>
+    <col min="10" max="10" width="13.46484375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="18" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" style="9" customWidth="1"/>
+    <col min="14" max="14" width="9.796875" style="10" customWidth="1"/>
+    <col min="15" max="15" width="24.3984375" style="9" customWidth="1"/>
+    <col min="16" max="16" width="18.3984375" style="9" customWidth="1"/>
+    <col min="17" max="17" width="18" style="9" customWidth="1"/>
+    <col min="18" max="18" width="25.06640625" style="9" customWidth="1"/>
+    <col min="19" max="19" width="10.59765625" style="11" customWidth="1"/>
+    <col min="20" max="20" width="5.59765625" style="10" customWidth="1"/>
+    <col min="21" max="21" width="9.796875" style="9" customWidth="1"/>
+    <col min="22" max="16384" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="164" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" ht="164" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="51"/>
       <c r="B1" s="57"/>
       <c r="C1" s="55"/>
@@ -1161,40 +1169,41 @@
       <c r="G1" s="55"/>
       <c r="H1" s="55"/>
       <c r="I1" s="55"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="55"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="2"/>
-    </row>
-    <row r="2" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V1" s="2"/>
+    </row>
+    <row r="2" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="53" t="s">
         <v>65</v>
       </c>
@@ -1219,43 +1228,46 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="7">
         <v>1</v>
       </c>
-      <c r="L2" s="8">
+      <c r="M2" s="8">
         <v>2</v>
       </c>
-      <c r="M2" s="7">
+      <c r="N2" s="7">
         <v>3</v>
       </c>
-      <c r="N2" s="8">
+      <c r="O2" s="8">
         <v>4</v>
       </c>
-      <c r="O2" s="7">
+      <c r="P2" s="7">
         <v>5</v>
       </c>
-      <c r="P2" s="8">
+      <c r="Q2" s="8">
         <v>6</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="R2" s="7">
         <v>7</v>
       </c>
-      <c r="R2" s="8">
+      <c r="S2" s="8">
         <v>8</v>
       </c>
-      <c r="S2" s="7">
+      <c r="T2" s="7">
         <v>9</v>
       </c>
-      <c r="T2" s="8">
+      <c r="U2" s="8">
         <v>10</v>
       </c>
-      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -1266,7 +1278,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1283,22 +1295,23 @@
     <col min="6" max="6" width="17.19921875" style="9" customWidth="1"/>
     <col min="7" max="7" width="22.1328125" style="9" customWidth="1"/>
     <col min="8" max="8" width="6" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.73046875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="22.33203125" style="9" customWidth="1"/>
-    <col min="13" max="13" width="19.9296875" style="11" customWidth="1"/>
-    <col min="14" max="14" width="7.6640625" style="10" customWidth="1"/>
-    <col min="15" max="15" width="33.53125" style="11" customWidth="1"/>
-    <col min="16" max="16" width="15.53125" style="11" customWidth="1"/>
-    <col min="17" max="17" width="9.59765625" style="11" customWidth="1"/>
-    <col min="18" max="18" width="11.19921875" style="10" customWidth="1"/>
-    <col min="19" max="19" width="15.9296875" style="10" customWidth="1"/>
-    <col min="20" max="20" width="13.53125" style="11" customWidth="1"/>
-    <col min="21" max="16384" width="9.06640625" style="3"/>
+    <col min="9" max="9" width="6" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.73046875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="19.9296875" style="11" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" style="10" customWidth="1"/>
+    <col min="16" max="16" width="33.53125" style="11" customWidth="1"/>
+    <col min="17" max="17" width="15.53125" style="11" customWidth="1"/>
+    <col min="18" max="18" width="9.59765625" style="11" customWidth="1"/>
+    <col min="19" max="19" width="11.19921875" style="10" customWidth="1"/>
+    <col min="20" max="20" width="15.9296875" style="10" customWidth="1"/>
+    <col min="21" max="21" width="13.53125" style="11" customWidth="1"/>
+    <col min="22" max="16384" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="164" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="164" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="51"/>
       <c r="B1" s="48"/>
       <c r="C1" s="25"/>
@@ -1308,39 +1321,40 @@
       <c r="G1" s="25"/>
       <c r="H1" s="27"/>
       <c r="I1" s="27"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="27"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="53" t="s">
         <v>65</v>
       </c>
@@ -1366,82 +1380,85 @@
         <v>20</v>
       </c>
       <c r="I2" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="K2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="24">
+      <c r="L2" s="24">
         <v>1</v>
       </c>
-      <c r="L2" s="24">
+      <c r="M2" s="24">
         <v>2</v>
       </c>
-      <c r="M2" s="24">
+      <c r="N2" s="24">
         <v>3</v>
       </c>
-      <c r="N2" s="24">
+      <c r="O2" s="24">
         <v>4</v>
       </c>
-      <c r="O2" s="24">
+      <c r="P2" s="24">
         <v>5</v>
       </c>
-      <c r="P2" s="24">
+      <c r="Q2" s="24">
         <v>6</v>
       </c>
-      <c r="Q2" s="24">
+      <c r="R2" s="24">
         <v>7</v>
       </c>
-      <c r="R2" s="24">
+      <c r="S2" s="24">
         <v>8</v>
       </c>
-      <c r="S2" s="24">
+      <c r="T2" s="24">
         <v>9</v>
       </c>
-      <c r="T2" s="24">
+      <c r="U2" s="24">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B3" s="47"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B4" s="47"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B5" s="47"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B6" s="47"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B7" s="47"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B8" s="47"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B9" s="47"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B10" s="47"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B11" s="47"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B12" s="47"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B13" s="47"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B14" s="47"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B15" s="47"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B16" s="47"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">
@@ -1506,6 +1523,448 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AA32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.06640625" style="52"/>
+    <col min="2" max="2" width="24" style="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" style="9" customWidth="1"/>
+    <col min="10" max="10" width="13" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27" style="9" customWidth="1"/>
+    <col min="13" max="14" width="11.3984375" style="11" customWidth="1"/>
+    <col min="15" max="15" width="16.265625" style="11" customWidth="1"/>
+    <col min="16" max="16" width="17.265625" style="11" customWidth="1"/>
+    <col min="17" max="18" width="11.9296875" style="11" customWidth="1"/>
+    <col min="19" max="19" width="17.73046875" style="11" customWidth="1"/>
+    <col min="20" max="20" width="9.46484375" style="10" customWidth="1"/>
+    <col min="21" max="21" width="12.86328125" style="11" customWidth="1"/>
+    <col min="22" max="23" width="9.06640625" style="30"/>
+    <col min="24" max="25" width="9.9296875" style="30" customWidth="1"/>
+    <col min="26" max="26" width="9.06640625" style="30"/>
+    <col min="27" max="16384" width="9.06640625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="164" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="51"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+    </row>
+    <row r="2" spans="1:27" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="23">
+        <v>1</v>
+      </c>
+      <c r="M2" s="24">
+        <v>2</v>
+      </c>
+      <c r="N2" s="23">
+        <v>3</v>
+      </c>
+      <c r="O2" s="24">
+        <v>4</v>
+      </c>
+      <c r="P2" s="23">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="24">
+        <v>6</v>
+      </c>
+      <c r="R2" s="23">
+        <v>7</v>
+      </c>
+      <c r="S2" s="24">
+        <v>8</v>
+      </c>
+      <c r="T2" s="23">
+        <v>9</v>
+      </c>
+      <c r="U2" s="24">
+        <v>10</v>
+      </c>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B3" s="47"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B4" s="47"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B5" s="47"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B6" s="47"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B7" s="47"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B8" s="47"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B9" s="47"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B10" s="47"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B11" s="47"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B12" s="47"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B13" s="47"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B14" s="47"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B15" s="47"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B16" s="47"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B17" s="47"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B18" s="47"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B19" s="47"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B20" s="47"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B21" s="47"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B22" s="47"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B23" s="47"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B24" s="47"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B25" s="47"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B26" s="47"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B27" s="47"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B28" s="47"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B29" s="47"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B30" s="47"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B31" s="47"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B32" s="47"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:Z3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.06640625" style="52"/>
+    <col min="2" max="2" width="24" style="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" style="9" customWidth="1"/>
+    <col min="10" max="10" width="13" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.46484375" style="9" customWidth="1"/>
+    <col min="14" max="14" width="12" style="10" customWidth="1"/>
+    <col min="15" max="15" width="6.19921875" style="10" customWidth="1"/>
+    <col min="16" max="16" width="6" style="10" customWidth="1"/>
+    <col min="17" max="21" width="11.06640625" style="11" customWidth="1"/>
+    <col min="22" max="23" width="9.06640625" style="30"/>
+    <col min="24" max="25" width="9.9296875" style="30" customWidth="1"/>
+    <col min="26" max="26" width="9.06640625" style="30"/>
+    <col min="27" max="16384" width="9.06640625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="9" customFormat="1" ht="164" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="51"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+    </row>
+    <row r="2" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="24">
+        <v>1</v>
+      </c>
+      <c r="M2" s="24">
+        <v>2</v>
+      </c>
+      <c r="N2" s="24">
+        <v>3</v>
+      </c>
+      <c r="O2" s="24">
+        <v>4</v>
+      </c>
+      <c r="P2" s="24">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="24">
+        <v>6</v>
+      </c>
+      <c r="R2" s="24">
+        <v>7</v>
+      </c>
+      <c r="S2" s="24">
+        <v>8</v>
+      </c>
+      <c r="T2" s="24">
+        <v>9</v>
+      </c>
+      <c r="U2" s="24">
+        <v>10</v>
+      </c>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="B3" s="49"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1522,20 +1981,18 @@
     <col min="5" max="5" width="6" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="17" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27" style="9" customWidth="1"/>
-    <col min="12" max="13" width="11.3984375" style="11" customWidth="1"/>
-    <col min="14" max="14" width="16.265625" style="11" customWidth="1"/>
-    <col min="15" max="15" width="17.265625" style="11" customWidth="1"/>
-    <col min="16" max="17" width="11.9296875" style="11" customWidth="1"/>
-    <col min="18" max="18" width="17.73046875" style="11" customWidth="1"/>
-    <col min="19" max="19" width="9.46484375" style="10" customWidth="1"/>
-    <col min="20" max="20" width="12.86328125" style="11" customWidth="1"/>
-    <col min="21" max="22" width="9.06640625" style="30"/>
-    <col min="23" max="24" width="9.9296875" style="30" customWidth="1"/>
-    <col min="25" max="25" width="9.06640625" style="30"/>
-    <col min="26" max="16384" width="9.06640625" style="3"/>
+    <col min="9" max="9" width="6" style="9" customWidth="1"/>
+    <col min="10" max="10" width="13" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.53125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="19.53125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="10.86328125" style="11" customWidth="1"/>
+    <col min="15" max="16" width="6.46484375" style="10" customWidth="1"/>
+    <col min="17" max="21" width="10.3984375" style="11" customWidth="1"/>
+    <col min="22" max="23" width="9.06640625" style="30"/>
+    <col min="24" max="25" width="9.9296875" style="30" customWidth="1"/>
+    <col min="26" max="26" width="9.06640625" style="30"/>
+    <col min="27" max="16384" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="164" customHeight="1" x14ac:dyDescent="0.45">
@@ -1547,46 +2004,46 @@
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="28" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-    </row>
-    <row r="2" spans="1:26" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="U1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="2"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A2" s="53" t="s">
         <v>65</v>
       </c>
@@ -1611,72 +2068,74 @@
       <c r="H2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="K2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="23">
+      <c r="L2" s="24">
         <v>1</v>
       </c>
-      <c r="L2" s="24">
+      <c r="M2" s="24">
         <v>2</v>
       </c>
-      <c r="M2" s="23">
+      <c r="N2" s="36">
         <v>3</v>
       </c>
-      <c r="N2" s="24">
+      <c r="O2" s="24">
         <v>4</v>
       </c>
-      <c r="O2" s="23">
+      <c r="P2" s="24">
         <v>5</v>
       </c>
-      <c r="P2" s="24">
+      <c r="Q2" s="36">
         <v>6</v>
       </c>
-      <c r="Q2" s="23">
+      <c r="R2" s="36">
         <v>7</v>
       </c>
-      <c r="R2" s="24">
+      <c r="S2" s="36">
         <v>8</v>
       </c>
-      <c r="S2" s="23">
+      <c r="T2" s="36">
         <v>9</v>
       </c>
-      <c r="T2" s="24">
+      <c r="U2" s="36">
         <v>10</v>
       </c>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="29"/>
-      <c r="Z2" s="29"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.45">
       <c r="B3" s="47"/>
-      <c r="U3" s="3"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.45">
       <c r="B4" s="47"/>
-      <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.45">
       <c r="B5" s="47"/>
-      <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.45">
       <c r="B6" s="47"/>
@@ -1709,432 +2168,6 @@
       <c r="B15" s="47"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="B16" s="47"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B17" s="47"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B18" s="47"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B19" s="47"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B20" s="47"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B21" s="47"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B22" s="47"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B23" s="47"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B24" s="47"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B25" s="47"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B26" s="47"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B27" s="47"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B28" s="47"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B29" s="47"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B30" s="47"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B31" s="47"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B32" s="47"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Y3"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="9.06640625" style="52"/>
-    <col min="2" max="2" width="24" style="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.46484375" style="9" customWidth="1"/>
-    <col min="13" max="13" width="12" style="10" customWidth="1"/>
-    <col min="14" max="14" width="6.19921875" style="10" customWidth="1"/>
-    <col min="15" max="15" width="6" style="10" customWidth="1"/>
-    <col min="16" max="20" width="11.06640625" style="11" customWidth="1"/>
-    <col min="21" max="22" width="9.06640625" style="30"/>
-    <col min="23" max="24" width="9.9296875" style="30" customWidth="1"/>
-    <col min="25" max="25" width="9.06640625" style="30"/>
-    <col min="26" max="16384" width="9.06640625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" s="9" customFormat="1" ht="164" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="51"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="S1" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-    </row>
-    <row r="2" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="24">
-        <v>1</v>
-      </c>
-      <c r="L2" s="24">
-        <v>2</v>
-      </c>
-      <c r="M2" s="24">
-        <v>3</v>
-      </c>
-      <c r="N2" s="24">
-        <v>4</v>
-      </c>
-      <c r="O2" s="24">
-        <v>5</v>
-      </c>
-      <c r="P2" s="24">
-        <v>6</v>
-      </c>
-      <c r="Q2" s="24">
-        <v>7</v>
-      </c>
-      <c r="R2" s="24">
-        <v>8</v>
-      </c>
-      <c r="S2" s="24">
-        <v>9</v>
-      </c>
-      <c r="T2" s="24">
-        <v>10</v>
-      </c>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="B3" s="49"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="34"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Y32"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="9.06640625" style="52"/>
-    <col min="2" max="2" width="24" style="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.53125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="19.53125" style="9" customWidth="1"/>
-    <col min="13" max="13" width="10.86328125" style="11" customWidth="1"/>
-    <col min="14" max="15" width="6.46484375" style="10" customWidth="1"/>
-    <col min="16" max="20" width="10.3984375" style="11" customWidth="1"/>
-    <col min="21" max="22" width="9.06640625" style="30"/>
-    <col min="23" max="24" width="9.9296875" style="30" customWidth="1"/>
-    <col min="25" max="25" width="9.06640625" style="30"/>
-    <col min="26" max="16384" width="9.06640625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" ht="164" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="51"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" s="2"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A2" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="24">
-        <v>1</v>
-      </c>
-      <c r="L2" s="24">
-        <v>2</v>
-      </c>
-      <c r="M2" s="36">
-        <v>3</v>
-      </c>
-      <c r="N2" s="24">
-        <v>4</v>
-      </c>
-      <c r="O2" s="24">
-        <v>5</v>
-      </c>
-      <c r="P2" s="36">
-        <v>6</v>
-      </c>
-      <c r="Q2" s="36">
-        <v>7</v>
-      </c>
-      <c r="R2" s="36">
-        <v>8</v>
-      </c>
-      <c r="S2" s="36">
-        <v>9</v>
-      </c>
-      <c r="T2" s="36">
-        <v>10</v>
-      </c>
-      <c r="U2" s="2"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B3" s="47"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B4" s="47"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B5" s="47"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B6" s="47"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B7" s="47"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B8" s="47"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B9" s="47"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B10" s="47"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B11" s="47"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B12" s="47"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B13" s="47"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B14" s="47"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="B15" s="47"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="B16" s="47"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">
@@ -2193,7 +2226,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -2210,21 +2243,22 @@
     <col min="6" max="6" width="16" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.59765625" style="11" customWidth="1"/>
-    <col min="14" max="14" width="13.3984375" style="11" customWidth="1"/>
-    <col min="15" max="15" width="6.19921875" style="10" customWidth="1"/>
-    <col min="16" max="16" width="6.46484375" style="10" customWidth="1"/>
-    <col min="17" max="17" width="11.796875" style="11" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" style="11" customWidth="1"/>
-    <col min="19" max="20" width="9.9296875" style="30" customWidth="1"/>
-    <col min="21" max="21" width="9.06640625" style="30"/>
-    <col min="22" max="16384" width="9.06640625" style="3"/>
+    <col min="9" max="9" width="6" style="9" customWidth="1"/>
+    <col min="10" max="10" width="13" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.59765625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="13.3984375" style="11" customWidth="1"/>
+    <col min="16" max="16" width="6.19921875" style="10" customWidth="1"/>
+    <col min="17" max="17" width="6.46484375" style="10" customWidth="1"/>
+    <col min="18" max="18" width="11.796875" style="11" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" style="11" customWidth="1"/>
+    <col min="20" max="21" width="9.9296875" style="30" customWidth="1"/>
+    <col min="22" max="22" width="9.06640625" style="30"/>
+    <col min="23" max="16384" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="164" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" ht="164" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="51"/>
       <c r="B1" s="48"/>
       <c r="C1" s="25"/>
@@ -2233,37 +2267,38 @@
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="1" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="S1" s="37"/>
-      <c r="T1" s="3"/>
+      <c r="T1" s="37"/>
       <c r="U1" s="3"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="V1" s="3"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A2" s="53" t="s">
         <v>65</v>
       </c>
@@ -2288,41 +2323,44 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="38">
+      <c r="L2" s="38">
         <v>1</v>
       </c>
-      <c r="L2" s="39">
+      <c r="M2" s="39">
         <v>2</v>
       </c>
-      <c r="M2" s="39">
+      <c r="N2" s="39">
         <v>3</v>
       </c>
-      <c r="N2" s="39">
+      <c r="O2" s="39">
         <v>4</v>
       </c>
-      <c r="O2" s="39">
+      <c r="P2" s="39">
         <v>5</v>
       </c>
-      <c r="P2" s="39">
+      <c r="Q2" s="39">
         <v>6</v>
       </c>
-      <c r="Q2" s="39">
+      <c r="R2" s="39">
         <v>7</v>
       </c>
-      <c r="R2" s="39">
+      <c r="S2" s="39">
         <v>8</v>
       </c>
-      <c r="S2" s="37"/>
-      <c r="T2" s="3"/>
+      <c r="T2" s="37"/>
       <c r="U2" s="3"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B3" s="50"/>
       <c r="C3" s="33"/>
       <c r="D3" s="34"/>
@@ -2330,55 +2368,56 @@
       <c r="F3" s="33"/>
       <c r="G3" s="33"/>
       <c r="H3" s="33"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="33"/>
-      <c r="S3" s="3"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="33"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="V3" s="3"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B4" s="47"/>
-      <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="V4" s="3"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B5" s="47"/>
-      <c r="S5" s="3"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="V5" s="3"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B6" s="47"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B7" s="47"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B8" s="47"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B9" s="47"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B10" s="47"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B11" s="47"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B12" s="47"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B13" s="47"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B14" s="47"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B15" s="47"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B16" s="47"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">

</xml_diff>